<commit_message>
add tests and fixes part 4
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/MIDAR_TestData_MHQuant_S1P_metadata_tables.xlsx
+++ b/tests/testthat/testdata/MIDAR_TestData_MHQuant_S1P_metadata_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10105"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lsibjb/Documents/Code/midar/tests/testthat/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C0194D-297E-FC4A-A056-53619ACA6E10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F28C37-4B07-3C4F-94E6-30214D2863B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8380" yWindow="5180" windowWidth="38120" windowHeight="22160" firstSheet="2" activeTab="13" xr2:uid="{7A04E2C8-868F-5640-98CB-88D372530A12}"/>
+    <workbookView xWindow="8380" yWindow="5180" windowWidth="38120" windowHeight="22160" activeTab="1" xr2:uid="{7A04E2C8-868F-5640-98CB-88D372530A12}"/>
   </bookViews>
   <sheets>
     <sheet name="Analyses" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1529" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1545" uniqueCount="136">
   <si>
     <t>analysis_id</t>
   </si>
@@ -424,15 +424,6 @@
     <t>S1P d19:1 [M&gt;113]</t>
   </si>
   <si>
-    <t>S1P d18:1 [M&gt;60]</t>
-  </si>
-  <si>
-    <t>S1P d18:2 [M&gt;60]</t>
-  </si>
-  <si>
-    <t>S1P d18:0 [M&gt;60]</t>
-  </si>
-  <si>
     <t>concentration</t>
   </si>
   <si>
@@ -452,13 +443,49 @@
   </si>
   <si>
     <t>S1P d18:1 [M&gt;213]</t>
+  </si>
+  <si>
+    <t>analyte_id</t>
+  </si>
+  <si>
+    <t>S1P d18:1</t>
+  </si>
+  <si>
+    <t>S1P d18:2</t>
+  </si>
+  <si>
+    <t>S1P d18:3</t>
+  </si>
+  <si>
+    <t>S1P d18:0</t>
+  </si>
+  <si>
+    <t>S1P d16:1</t>
+  </si>
+  <si>
+    <t>S1P d17:1</t>
+  </si>
+  <si>
+    <t>S1P d18:0</t>
+  </si>
+  <si>
+    <t>S1P d18:1</t>
+  </si>
+  <si>
+    <t>S1P d18:2</t>
+  </si>
+  <si>
+    <t>S1P d19:1</t>
+  </si>
+  <si>
+    <t>S1P d20:1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -610,6 +637,12 @@
       <color rgb="FF000000"/>
       <name val="Lucida Grande"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -5620,10 +5653,10 @@
         <v>19</v>
       </c>
       <c r="F1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H1" t="s">
         <v>22</v>
@@ -5950,10 +5983,10 @@
         <v>19</v>
       </c>
       <c r="F1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H1" t="s">
         <v>22</v>
@@ -6355,7 +6388,7 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="I4">
         <v>3.1587200000000003E-2</v>
@@ -6527,7 +6560,7 @@
         <v>1</v>
       </c>
       <c r="H12" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I12">
         <v>2.8666500000000001E-2</v>
@@ -6628,7 +6661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{391E718A-19CC-B043-9E91-EBD4CD5DE280}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -6995,10 +7028,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA4946AB-D291-A441-8BD4-AFE744BDE9E2}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="A1:J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7006,7 +7039,7 @@
     <col min="1" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -7020,25 +7053,28 @@
         <v>18</v>
       </c>
       <c r="E1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
-        <v>20</v>
-      </c>
       <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>22</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>23</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>101</v>
       </c>
@@ -7048,17 +7084,20 @@
       <c r="C2" t="s">
         <v>103</v>
       </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" t="b">
+      <c r="E2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>104</v>
       </c>
@@ -7068,17 +7107,20 @@
       <c r="C3" t="s">
         <v>103</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" t="b">
+      <c r="E3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3">
         <v>1</v>
       </c>
       <c r="G3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>105</v>
       </c>
@@ -7088,23 +7130,26 @@
       <c r="C4" t="s">
         <v>103</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" t="b">
+      <c r="E4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" t="b">
         <v>1</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
         <v>106</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>3.1587200000000003E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>106</v>
       </c>
@@ -7114,23 +7159,26 @@
       <c r="C5" t="s">
         <v>103</v>
       </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" t="b">
+      <c r="E5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F5">
         <v>1</v>
       </c>
       <c r="G5" t="b">
         <v>1</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
         <v>107</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>3.1538499999999997E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>102</v>
       </c>
@@ -7140,17 +7188,20 @@
       <c r="C6" t="s">
         <v>103</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6" t="b">
+      <c r="E6" t="s">
+        <v>132</v>
+      </c>
+      <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>107</v>
       </c>
@@ -7160,17 +7211,20 @@
       <c r="C7" t="s">
         <v>103</v>
       </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7" t="b">
+      <c r="E7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F7">
         <v>1</v>
       </c>
       <c r="G7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>108</v>
       </c>
@@ -7180,17 +7234,20 @@
       <c r="C8" t="s">
         <v>103</v>
       </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8" t="b">
+      <c r="E8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>109</v>
       </c>
@@ -7200,17 +7257,20 @@
       <c r="C9" t="s">
         <v>103</v>
       </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9" t="b">
+      <c r="E9" t="s">
+        <v>135</v>
+      </c>
+      <c r="F9">
         <v>1</v>
       </c>
       <c r="G9" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>110</v>
       </c>
@@ -7220,17 +7280,20 @@
       <c r="C10" t="s">
         <v>103</v>
       </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10" t="b">
+      <c r="E10" t="s">
+        <v>129</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="b">
         <v>0</v>
       </c>
-      <c r="G10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>112</v>
       </c>
@@ -7240,17 +7303,20 @@
       <c r="C11" t="s">
         <v>103</v>
       </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11" t="b">
+      <c r="E11" t="s">
+        <v>130</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="b">
         <v>0</v>
       </c>
-      <c r="G11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>113</v>
       </c>
@@ -7260,23 +7326,26 @@
       <c r="C12" t="s">
         <v>103</v>
       </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12" t="b">
+      <c r="E12" t="s">
+        <v>131</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" t="b">
         <v>0</v>
       </c>
-      <c r="G12" t="b">
-        <v>1</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="H12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" t="s">
         <v>114</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>2.8666500000000001E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>114</v>
       </c>
@@ -7286,23 +7355,26 @@
       <c r="C13" t="s">
         <v>103</v>
       </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13" t="b">
+      <c r="E13" t="s">
+        <v>132</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="b">
         <v>0</v>
       </c>
-      <c r="G13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H13" t="s">
+      <c r="H13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" t="s">
         <v>115</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>2.86123E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>111</v>
       </c>
@@ -7312,17 +7384,20 @@
       <c r="C14" t="s">
         <v>103</v>
       </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14" t="b">
+      <c r="E14" t="s">
+        <v>132</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="b">
         <v>0</v>
       </c>
-      <c r="G14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>115</v>
       </c>
@@ -7332,17 +7407,20 @@
       <c r="C15" t="s">
         <v>103</v>
       </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15" t="b">
+      <c r="E15" t="s">
+        <v>133</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" t="b">
         <v>0</v>
       </c>
-      <c r="G15" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>116</v>
       </c>
@@ -7352,13 +7430,16 @@
       <c r="C16" t="s">
         <v>103</v>
       </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16" t="b">
+      <c r="E16" t="s">
+        <v>134</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="b">
         <v>0</v>
       </c>
-      <c r="G16" t="b">
+      <c r="H16" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7619,7 +7700,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="A2:B7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7633,13 +7714,13 @@
         <v>98</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>124</v>
       </c>
       <c r="C1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E1" t="s">
         <v>24</v>
@@ -7650,13 +7731,13 @@
         <v>88</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="C2">
         <v>0.2</v>
       </c>
       <c r="D2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -7664,13 +7745,13 @@
         <v>87</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="C3">
         <v>0.2</v>
       </c>
       <c r="D3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -7678,13 +7759,13 @@
         <v>88</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="C4">
         <v>0.1</v>
       </c>
       <c r="D4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -7692,13 +7773,13 @@
         <v>87</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="C5">
         <v>0.1</v>
       </c>
       <c r="D5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -7706,13 +7787,13 @@
         <v>88</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="C6">
         <v>0.05</v>
       </c>
       <c r="D6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -7720,16 +7801,17 @@
         <v>87</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="C7">
         <v>0.05</v>
       </c>
       <c r="D7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="21" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -9752,10 +9834,10 @@
         <v>19</v>
       </c>
       <c r="F1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H1" t="s">
         <v>22</v>
@@ -10082,10 +10164,10 @@
         <v>19</v>
       </c>
       <c r="F1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H1" t="s">
         <v>22</v>
@@ -10448,10 +10530,10 @@
         <v>19</v>
       </c>
       <c r="F1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H1" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
fix interference_contribution in templates
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/MIDAR_TestData_MHQuant_S1P_metadata_tables.xlsx
+++ b/tests/testthat/testdata/MIDAR_TestData_MHQuant_S1P_metadata_tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10407"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lsibjb/Documents/Code/midar/tests/testthat/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F28C37-4B07-3C4F-94E6-30214D2863B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE9D0A5B-3AC6-2B47-8BB3-8CFF991FEDB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8380" yWindow="5180" windowWidth="38120" windowHeight="22160" activeTab="1" xr2:uid="{7A04E2C8-868F-5640-98CB-88D372530A12}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1545" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1545" uniqueCount="137">
   <si>
     <t>analysis_id</t>
   </si>
@@ -479,6 +479,9 @@
   </si>
   <si>
     <t>S1P d20:1</t>
+  </si>
+  <si>
+    <t>interference_contribution</t>
   </si>
 </sst>
 </file>
@@ -7031,7 +7034,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7068,7 +7071,7 @@
         <v>22</v>
       </c>
       <c r="J1" t="s">
-        <v>23</v>
+        <v>136</v>
       </c>
       <c r="K1" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
support mass concentrations and postprocessed data
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/MIDAR_TestData_MHQuant_S1P_metadata_tables.xlsx
+++ b/tests/testthat/testdata/MIDAR_TestData_MHQuant_S1P_metadata_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10407"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lsibjb/Documents/Code/midar/tests/testthat/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F28C37-4B07-3C4F-94E6-30214D2863B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E0E57D-74DD-0F49-B3E0-2E8C94EDCEAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8380" yWindow="5180" windowWidth="38120" windowHeight="22160" activeTab="1" xr2:uid="{7A04E2C8-868F-5640-98CB-88D372530A12}"/>
+    <workbookView xWindow="8380" yWindow="5180" windowWidth="38120" windowHeight="22160" activeTab="2" xr2:uid="{7A04E2C8-868F-5640-98CB-88D372530A12}"/>
   </bookViews>
   <sheets>
     <sheet name="Analyses" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1545" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1546" uniqueCount="137">
   <si>
     <t>analysis_id</t>
   </si>
@@ -479,6 +479,9 @@
   </si>
   <si>
     <t>S1P d20:1</t>
+  </si>
+  <si>
+    <t>istd_conc_ngml</t>
   </si>
 </sst>
 </file>
@@ -7030,7 +7033,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA4946AB-D291-A441-8BD4-AFE744BDE9E2}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -7450,10 +7453,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CEF20C9-E726-8549-8B20-6F3F3BE0DDC1}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7461,7 +7464,7 @@
     <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -7469,10 +7472,13 @@
         <v>25</v>
       </c>
       <c r="C1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>102</v>
       </c>
@@ -7480,7 +7486,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>111</v>
       </c>

</xml_diff>